<commit_message>
Making PC figures of 251
</commit_message>
<xml_diff>
--- a/meta/BMAG069_Suckers_2021_Barcodes_01062021.xlsx
+++ b/meta/BMAG069_Suckers_2021_Barcodes_01062021.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="0" windowWidth="25360" windowHeight="15360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Barcodes" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5979" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5979" uniqueCount="740">
   <si>
     <t>Sample ID</t>
   </si>
@@ -2243,14 +2243,84 @@
   <si>
     <t>lacuanserinus</t>
   </si>
+  <si>
+    <t>KSS_3734-017</t>
+  </si>
+  <si>
+    <r>
+      <t>KSS_3734-01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>KSS_3734-01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>KSS_3734-01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>KSS_3734-01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2520,228 +2590,232 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2754,57 +2828,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2835,6 +2910,8 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2865,6 +2942,8 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -3149,8 +3228,8 @@
   </sheetPr>
   <dimension ref="A1:H316"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="A310" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11096,7 +11175,7 @@
     </row>
     <row r="306" spans="1:8">
       <c r="A306" s="68" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="B306" s="76" t="s">
         <v>102</v>
@@ -11122,7 +11201,7 @@
     </row>
     <row r="307" spans="1:8">
       <c r="A307" s="68" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="B307" s="76" t="s">
         <v>102</v>
@@ -11148,7 +11227,7 @@
     </row>
     <row r="308" spans="1:8">
       <c r="A308" s="71" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="B308" s="76" t="s">
         <v>102</v>
@@ -11174,7 +11253,7 @@
     </row>
     <row r="309" spans="1:8" ht="15" thickBot="1">
       <c r="A309" s="74" t="s">
-        <v>478</v>
+        <v>735</v>
       </c>
       <c r="B309" s="77" t="s">
         <v>102</v>
@@ -11266,8 +11345,8 @@
   </sheetPr>
   <dimension ref="A1:P309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D98" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="A310" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22625,8 +22704,8 @@
       </c>
     </row>
     <row r="306" spans="1:14">
-      <c r="A306" s="14" t="s">
-        <v>442</v>
+      <c r="A306" s="82" t="s">
+        <v>736</v>
       </c>
       <c r="D306" s="59" t="s">
         <v>687</v>
@@ -22655,8 +22734,8 @@
       </c>
     </row>
     <row r="307" spans="1:14">
-      <c r="A307" s="14" t="s">
-        <v>454</v>
+      <c r="A307" s="82" t="s">
+        <v>737</v>
       </c>
       <c r="D307" s="59" t="s">
         <v>687</v>
@@ -22685,8 +22764,8 @@
       </c>
     </row>
     <row r="308" spans="1:14">
-      <c r="A308" s="14" t="s">
-        <v>466</v>
+      <c r="A308" s="82" t="s">
+        <v>738</v>
       </c>
       <c r="D308" s="59" t="s">
         <v>687</v>
@@ -22715,8 +22794,8 @@
       </c>
     </row>
     <row r="309" spans="1:14">
-      <c r="A309" s="14" t="s">
-        <v>478</v>
+      <c r="A309" s="82" t="s">
+        <v>739</v>
       </c>
       <c r="D309" s="59" t="s">
         <v>687</v>

</xml_diff>